<commit_message>
change table database in excel
</commit_message>
<xml_diff>
--- a/analisa/analisa siakes.xlsx
+++ b/analisa/analisa siakes.xlsx
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="153">
   <si>
     <t>admin</t>
   </si>
@@ -402,15 +402,9 @@
     <t>tb_guru</t>
   </si>
   <si>
-    <t>tb_guru_history</t>
-  </si>
-  <si>
     <t>nik</t>
   </si>
   <si>
-    <t>id_guru</t>
-  </si>
-  <si>
     <t>guru01</t>
   </si>
   <si>
@@ -625,9 +619,6 @@
   </si>
   <si>
     <t>Subsidi B</t>
-  </si>
-  <si>
-    <t>id_hp</t>
   </si>
   <si>
     <t>is_manual</t>
@@ -1108,12 +1099,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1145,6 +1130,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1369,8 +1360,8 @@
   </sheetPr>
   <dimension ref="A1:AH1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:L58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1527,10 +1518,10 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="76"/>
+      <c r="B13" s="87"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
@@ -1545,7 +1536,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G14" s="10"/>
       <c r="J14" s="3"/>
@@ -1589,19 +1580,19 @@
         <v>25</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>27</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="K15" s="84" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K15" s="82" t="s">
+        <v>97</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
@@ -1639,23 +1630,23 @@
         <v>1</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H16" s="5">
         <v>1</v>
       </c>
-      <c r="I16" s="77">
+      <c r="I16" s="75">
         <v>200000</v>
       </c>
       <c r="J16" s="16">
         <v>1</v>
       </c>
-      <c r="K16" s="85">
+      <c r="K16" s="83">
         <f>I16*J16</f>
         <v>200000</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N16" s="56"/>
       <c r="O16" s="9"/>
@@ -1693,23 +1684,23 @@
         <v>2</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H17" s="5">
         <v>1</v>
       </c>
-      <c r="I17" s="77">
+      <c r="I17" s="75">
         <v>150000</v>
       </c>
       <c r="J17" s="16">
         <v>1</v>
       </c>
-      <c r="K17" s="85">
+      <c r="K17" s="83">
         <f t="shared" ref="K17:K58" si="0">I17*J17</f>
         <v>150000</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N17" s="56"/>
       <c r="O17" s="57"/>
@@ -1747,23 +1738,23 @@
         <v>3</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H18" s="5">
         <v>1</v>
       </c>
-      <c r="I18" s="77">
+      <c r="I18" s="75">
         <v>100000</v>
       </c>
       <c r="J18" s="16">
         <v>1</v>
       </c>
-      <c r="K18" s="85">
+      <c r="K18" s="83">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N18" s="56"/>
       <c r="O18" s="57"/>
@@ -1801,23 +1792,23 @@
         <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H19" s="5">
         <v>1</v>
       </c>
-      <c r="I19" s="77">
+      <c r="I19" s="75">
         <v>150000</v>
       </c>
       <c r="J19" s="16">
         <v>1</v>
       </c>
-      <c r="K19" s="85">
+      <c r="K19" s="83">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N19" s="56"/>
       <c r="O19" s="9"/>
@@ -1855,23 +1846,23 @@
         <v>5</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H20" s="5">
         <v>1</v>
       </c>
-      <c r="I20" s="77">
+      <c r="I20" s="75">
         <v>200000</v>
       </c>
       <c r="J20" s="16">
         <v>1</v>
       </c>
-      <c r="K20" s="85">
+      <c r="K20" s="83">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N20" s="47"/>
       <c r="O20" s="57"/>
@@ -1900,7 +1891,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>9</v>
@@ -1914,18 +1905,18 @@
       <c r="H21" s="5">
         <v>1</v>
       </c>
-      <c r="I21" s="77">
+      <c r="I21" s="75">
         <v>700000</v>
       </c>
       <c r="J21" s="16">
         <v>1</v>
       </c>
-      <c r="K21" s="85">
+      <c r="K21" s="83">
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N21" s="47"/>
       <c r="O21" s="9"/>
@@ -1954,7 +1945,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>9</v>
@@ -1968,18 +1959,18 @@
       <c r="H22" s="5">
         <v>1</v>
       </c>
-      <c r="I22" s="77">
+      <c r="I22" s="75">
         <v>60000</v>
       </c>
       <c r="J22" s="21">
         <v>12</v>
       </c>
-      <c r="K22" s="85">
+      <c r="K22" s="83">
         <f t="shared" si="0"/>
         <v>720000</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N22" s="47"/>
       <c r="O22" s="9"/>
@@ -2008,7 +1999,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>9</v>
@@ -2022,18 +2013,18 @@
       <c r="H23" s="5">
         <v>1</v>
       </c>
-      <c r="I23" s="77">
+      <c r="I23" s="75">
         <v>100000</v>
       </c>
       <c r="J23" s="21">
         <v>1</v>
       </c>
-      <c r="K23" s="85">
+      <c r="K23" s="83">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N23" s="47"/>
       <c r="O23" s="57"/>
@@ -2062,7 +2053,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>10</v>
@@ -2076,18 +2067,18 @@
       <c r="H24" s="5">
         <v>1</v>
       </c>
-      <c r="I24" s="77">
+      <c r="I24" s="75">
         <v>100000</v>
       </c>
       <c r="J24" s="21">
         <v>1</v>
       </c>
-      <c r="K24" s="85">
+      <c r="K24" s="83">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N24" s="47"/>
       <c r="O24" s="57"/>
@@ -2116,7 +2107,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>10</v>
@@ -2130,18 +2121,18 @@
       <c r="H25" s="5">
         <v>1</v>
       </c>
-      <c r="I25" s="77">
+      <c r="I25" s="75">
         <v>50000</v>
       </c>
       <c r="J25" s="21">
         <v>1</v>
       </c>
-      <c r="K25" s="85">
+      <c r="K25" s="83">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N25" s="47"/>
       <c r="O25" s="9"/>
@@ -2170,7 +2161,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>10</v>
@@ -2184,18 +2175,18 @@
       <c r="H26" s="5">
         <v>1</v>
       </c>
-      <c r="I26" s="77">
+      <c r="I26" s="75">
         <v>60000</v>
       </c>
       <c r="J26" s="27">
         <v>12</v>
       </c>
-      <c r="K26" s="85">
+      <c r="K26" s="83">
         <f t="shared" si="0"/>
         <v>720000</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N26" s="47"/>
       <c r="O26" s="9"/>
@@ -2232,18 +2223,18 @@
       <c r="H27" s="5">
         <v>1</v>
       </c>
-      <c r="I27" s="77">
+      <c r="I27" s="75">
         <v>820000</v>
       </c>
       <c r="J27" s="27">
         <v>1</v>
       </c>
-      <c r="K27" s="85">
+      <c r="K27" s="83">
         <f t="shared" si="0"/>
         <v>820000</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2259,18 +2250,18 @@
       <c r="H28" s="5">
         <v>1</v>
       </c>
-      <c r="I28" s="77">
+      <c r="I28" s="75">
         <v>300000</v>
       </c>
       <c r="J28" s="27">
         <v>1</v>
       </c>
-      <c r="K28" s="85">
+      <c r="K28" s="83">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2283,23 +2274,23 @@
       <c r="H29" s="5">
         <v>1</v>
       </c>
-      <c r="I29" s="77">
+      <c r="I29" s="75">
         <v>100000</v>
       </c>
       <c r="J29" s="27">
         <v>1</v>
       </c>
-      <c r="K29" s="85">
+      <c r="K29" s="83">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F30" s="28">
         <v>11</v>
@@ -2310,18 +2301,18 @@
       <c r="H30" s="30">
         <v>1</v>
       </c>
-      <c r="I30" s="78">
+      <c r="I30" s="76">
         <v>100000</v>
       </c>
       <c r="J30" s="31">
         <v>1</v>
       </c>
-      <c r="K30" s="85">
+      <c r="K30" s="83">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2340,18 +2331,18 @@
       <c r="H31" s="18">
         <v>1</v>
       </c>
-      <c r="I31" s="79">
+      <c r="I31" s="77">
         <v>50000</v>
       </c>
       <c r="J31" s="33">
         <v>1</v>
       </c>
-      <c r="K31" s="85">
+      <c r="K31" s="83">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2365,23 +2356,23 @@
         <v>13</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H32" s="18">
         <v>1</v>
       </c>
-      <c r="I32" s="80">
+      <c r="I32" s="78">
         <v>250000</v>
       </c>
       <c r="J32" s="32">
         <v>1</v>
       </c>
-      <c r="K32" s="85">
+      <c r="K32" s="83">
         <f t="shared" si="0"/>
         <v>250000</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2395,23 +2386,23 @@
         <v>14</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H33" s="18">
         <v>1</v>
       </c>
-      <c r="I33" s="80">
+      <c r="I33" s="78">
         <v>600000</v>
       </c>
       <c r="J33" s="18">
         <v>1</v>
       </c>
-      <c r="K33" s="85">
+      <c r="K33" s="83">
         <f t="shared" si="0"/>
         <v>600000</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2424,45 +2415,45 @@
       <c r="H34" s="18">
         <v>1</v>
       </c>
-      <c r="I34" s="81">
+      <c r="I34" s="79">
         <v>300000</v>
       </c>
       <c r="J34" s="32">
         <v>1</v>
       </c>
-      <c r="K34" s="85">
+      <c r="K34" s="83">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F35" s="32">
         <v>16</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H35" s="18">
         <v>1</v>
       </c>
-      <c r="I35" s="82">
+      <c r="I35" s="80">
         <v>200000</v>
       </c>
       <c r="J35" s="18">
         <v>1</v>
       </c>
-      <c r="K35" s="86">
+      <c r="K35" s="84">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2470,35 +2461,35 @@
         <v>19</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C36" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="45" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F36" s="32">
         <v>17</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H36" s="18">
         <v>1</v>
       </c>
-      <c r="I36" s="82">
+      <c r="I36" s="80">
         <v>50000</v>
       </c>
       <c r="J36" s="32">
         <v>1</v>
       </c>
-      <c r="K36" s="86">
+      <c r="K36" s="84">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2509,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D37" s="18">
         <v>0</v>
@@ -2518,23 +2509,23 @@
         <v>18</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H37" s="18">
         <v>1</v>
       </c>
-      <c r="I37" s="82">
+      <c r="I37" s="80">
         <v>100000</v>
       </c>
       <c r="J37" s="18">
         <v>1</v>
       </c>
-      <c r="K37" s="86">
+      <c r="K37" s="84">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2545,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D38" s="18">
         <v>1</v>
@@ -2554,23 +2545,23 @@
         <v>19</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H38" s="18">
         <v>1</v>
       </c>
-      <c r="I38" s="82">
+      <c r="I38" s="80">
         <v>500000</v>
       </c>
       <c r="J38" s="32">
         <v>1</v>
       </c>
-      <c r="K38" s="86">
+      <c r="K38" s="84">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2590,23 +2581,23 @@
         <v>20</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H39" s="18">
         <v>1</v>
       </c>
-      <c r="I39" s="82">
+      <c r="I39" s="80">
         <v>100000</v>
       </c>
       <c r="J39" s="18">
         <v>1</v>
       </c>
-      <c r="K39" s="86">
+      <c r="K39" s="84">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="L39" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2617,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D40" s="18">
         <v>1</v>
@@ -2626,23 +2617,23 @@
         <v>21</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H40" s="18">
         <v>1</v>
       </c>
-      <c r="I40" s="82">
+      <c r="I40" s="80">
         <v>200000</v>
       </c>
       <c r="J40" s="32">
         <v>1</v>
       </c>
-      <c r="K40" s="86">
+      <c r="K40" s="84">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2653,7 +2644,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D41" s="18">
         <v>1</v>
@@ -2668,13 +2659,13 @@
       <c r="H41" s="50">
         <v>2</v>
       </c>
-      <c r="I41" s="83">
+      <c r="I41" s="81">
         <v>0</v>
       </c>
       <c r="J41" s="48">
         <v>1</v>
       </c>
-      <c r="K41" s="87">
+      <c r="K41" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2686,18 +2677,18 @@
         <v>23</v>
       </c>
       <c r="G42" s="51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H42" s="50">
         <v>2</v>
       </c>
-      <c r="I42" s="83">
+      <c r="I42" s="81">
         <v>0</v>
       </c>
       <c r="J42" s="48">
         <v>1</v>
       </c>
-      <c r="K42" s="87">
+      <c r="K42" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2709,18 +2700,18 @@
         <v>24</v>
       </c>
       <c r="G43" s="51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H43" s="50">
         <v>2</v>
       </c>
-      <c r="I43" s="83">
+      <c r="I43" s="81">
         <v>0</v>
       </c>
       <c r="J43" s="48">
         <v>1</v>
       </c>
-      <c r="K43" s="87">
+      <c r="K43" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2737,13 +2728,13 @@
       <c r="H44" s="18">
         <v>3</v>
       </c>
-      <c r="I44" s="79">
+      <c r="I44" s="77">
         <v>20000</v>
       </c>
       <c r="J44" s="32">
         <v>1</v>
       </c>
-      <c r="K44" s="86">
+      <c r="K44" s="84">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
@@ -2760,13 +2751,13 @@
       <c r="H45" s="18">
         <v>3</v>
       </c>
-      <c r="I45" s="79">
+      <c r="I45" s="77">
         <v>100000</v>
       </c>
       <c r="J45" s="32">
         <v>1</v>
       </c>
-      <c r="K45" s="86">
+      <c r="K45" s="84">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
@@ -2783,13 +2774,13 @@
       <c r="H46" s="18">
         <v>3</v>
       </c>
-      <c r="I46" s="79">
+      <c r="I46" s="77">
         <v>300000</v>
       </c>
       <c r="J46" s="32">
         <v>1</v>
       </c>
-      <c r="K46" s="86">
+      <c r="K46" s="84">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
@@ -2801,18 +2792,18 @@
         <v>28</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H47" s="18">
         <v>3</v>
       </c>
-      <c r="I47" s="79">
+      <c r="I47" s="77">
         <v>800000</v>
       </c>
       <c r="J47" s="32">
         <v>1</v>
       </c>
-      <c r="K47" s="86">
+      <c r="K47" s="84">
         <f t="shared" si="0"/>
         <v>800000</v>
       </c>
@@ -2829,13 +2820,13 @@
       <c r="H48" s="18">
         <v>3</v>
       </c>
-      <c r="I48" s="79">
+      <c r="I48" s="77">
         <v>400000</v>
       </c>
       <c r="J48" s="32">
         <v>1</v>
       </c>
-      <c r="K48" s="86">
+      <c r="K48" s="84">
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
@@ -2852,13 +2843,13 @@
       <c r="H49" s="18">
         <v>3</v>
       </c>
-      <c r="I49" s="79">
+      <c r="I49" s="77">
         <v>150000</v>
       </c>
       <c r="J49" s="32">
         <v>1</v>
       </c>
-      <c r="K49" s="86">
+      <c r="K49" s="84">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
@@ -2870,18 +2861,18 @@
         <v>31</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H50" s="18">
         <v>3</v>
       </c>
-      <c r="I50" s="79">
+      <c r="I50" s="77">
         <v>300000</v>
       </c>
       <c r="J50" s="32">
         <v>1</v>
       </c>
-      <c r="K50" s="86">
+      <c r="K50" s="84">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
@@ -2893,18 +2884,18 @@
         <v>32</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H51" s="18">
         <v>3</v>
       </c>
-      <c r="I51" s="79">
+      <c r="I51" s="77">
         <v>400000</v>
       </c>
       <c r="J51" s="32">
         <v>1</v>
       </c>
-      <c r="K51" s="86">
+      <c r="K51" s="84">
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
@@ -2916,18 +2907,18 @@
         <v>33</v>
       </c>
       <c r="G52" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H52" s="18">
         <v>3</v>
       </c>
-      <c r="I52" s="79">
+      <c r="I52" s="77">
         <v>130000</v>
       </c>
       <c r="J52" s="32">
         <v>1</v>
       </c>
-      <c r="K52" s="86">
+      <c r="K52" s="84">
         <f t="shared" si="0"/>
         <v>130000</v>
       </c>
@@ -2939,18 +2930,18 @@
         <v>34</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H53" s="18">
         <v>3</v>
       </c>
-      <c r="I53" s="79">
+      <c r="I53" s="77">
         <v>300000</v>
       </c>
       <c r="J53" s="32">
         <v>1</v>
       </c>
-      <c r="K53" s="86">
+      <c r="K53" s="84">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
@@ -2962,18 +2953,18 @@
         <v>35</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H54" s="18">
         <v>3</v>
       </c>
-      <c r="I54" s="79">
+      <c r="I54" s="77">
         <v>1000000</v>
       </c>
       <c r="J54" s="32">
         <v>1</v>
       </c>
-      <c r="K54" s="86">
+      <c r="K54" s="84">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
@@ -2985,18 +2976,18 @@
         <v>36</v>
       </c>
       <c r="G55" s="51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H55" s="50">
         <v>4</v>
       </c>
-      <c r="I55" s="83">
+      <c r="I55" s="81">
         <v>0</v>
       </c>
       <c r="J55" s="48">
         <v>1</v>
       </c>
-      <c r="K55" s="87">
+      <c r="K55" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3008,18 +2999,18 @@
         <v>37</v>
       </c>
       <c r="G56" s="51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H56" s="50">
         <v>4</v>
       </c>
-      <c r="I56" s="83">
+      <c r="I56" s="81">
         <v>0</v>
       </c>
       <c r="J56" s="48">
         <v>1</v>
       </c>
-      <c r="K56" s="87">
+      <c r="K56" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3031,18 +3022,18 @@
         <v>38</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H57" s="18">
         <v>5</v>
       </c>
-      <c r="I57" s="82">
+      <c r="I57" s="80">
         <v>0</v>
       </c>
       <c r="J57" s="32">
         <v>1</v>
       </c>
-      <c r="K57" s="86">
+      <c r="K57" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3054,18 +3045,18 @@
         <v>38</v>
       </c>
       <c r="G58" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H58" s="18">
         <v>5</v>
       </c>
-      <c r="I58" s="82">
+      <c r="I58" s="80">
         <v>0</v>
       </c>
       <c r="J58" s="32">
         <v>1</v>
       </c>
-      <c r="K58" s="86">
+      <c r="K58" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3252,120 +3243,122 @@
       <c r="E65" s="35"/>
       <c r="G65" s="35"/>
       <c r="H65" s="36"/>
-      <c r="M65" s="38" t="s">
-        <v>70</v>
-      </c>
+      <c r="M65" s="11"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
     </row>
     <row r="66" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D66" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="G66" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="H66" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H66" s="36"/>
-      <c r="M66" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N66" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="O66" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
     </row>
     <row r="67" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="22">
         <v>1</v>
       </c>
       <c r="B67" s="42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="D67" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" s="39">
+        <v>37310</v>
+      </c>
+      <c r="F67" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="E67" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="F67" s="40" t="s">
+      <c r="G67" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="H67" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="H67" s="36"/>
-      <c r="M67" s="22">
-        <v>1</v>
-      </c>
-      <c r="N67" s="22">
-        <v>1</v>
-      </c>
-      <c r="O67" s="22">
-        <v>1</v>
-      </c>
+      <c r="M67" s="47"/>
+      <c r="N67" s="47"/>
+      <c r="O67" s="47"/>
     </row>
     <row r="68" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="28">
         <v>2</v>
       </c>
       <c r="B68" s="59" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C68" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D68" s="28" t="s">
+      <c r="D68" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E68" s="39">
+        <v>37622</v>
+      </c>
+      <c r="F68" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E68" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="F68" s="60" t="s">
+      <c r="G68" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="H68" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="H68" s="36"/>
-      <c r="M68" s="22">
-        <v>2</v>
-      </c>
-      <c r="N68" s="22">
-        <v>1</v>
-      </c>
-      <c r="O68" s="22">
-        <v>2</v>
-      </c>
+      <c r="M68" s="47"/>
+      <c r="N68" s="47"/>
+      <c r="O68" s="47"/>
     </row>
     <row r="69" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="65">
         <v>3</v>
       </c>
       <c r="B69" s="59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C69" s="66" t="s">
-        <v>73</v>
-      </c>
-      <c r="D69" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E69" s="39">
+        <v>37623</v>
+      </c>
+      <c r="F69" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E69" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="F69" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="H69" s="36"/>
+      <c r="G69" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="H69" s="60" t="s">
+        <v>138</v>
+      </c>
       <c r="M69" s="26"/>
       <c r="N69" s="26"/>
       <c r="O69" s="26"/>
@@ -3375,21 +3368,26 @@
         <v>4</v>
       </c>
       <c r="B70" s="61" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D70" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="39">
+        <v>37624</v>
+      </c>
+      <c r="F70" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="E70" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F70" s="62" t="s">
-        <v>141</v>
-      </c>
-      <c r="H70" s="36"/>
+      <c r="G70" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="H70" s="62" t="s">
+        <v>139</v>
+      </c>
       <c r="M70" s="26"/>
       <c r="N70" s="26"/>
       <c r="O70" s="26"/>
@@ -3402,7 +3400,7 @@
     </row>
     <row r="72" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E72" s="2"/>
       <c r="K72" s="43"/>
@@ -3412,25 +3410,25 @@
         <v>19</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D73" s="4" t="s">
+      <c r="F73" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="G73" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="H73" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="L73" s="43"/>
     </row>
@@ -3466,7 +3464,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C75" s="5">
         <v>1</v>
@@ -3475,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F75" s="69"/>
       <c r="G75" s="69"/>
@@ -3495,7 +3493,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="52" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F76" s="70">
         <v>150000</v>
@@ -3513,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C77" s="18">
         <v>2</v>
@@ -3522,7 +3520,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F77" s="71"/>
       <c r="G77" s="71"/>
@@ -3534,7 +3532,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C78" s="18">
         <v>2</v>
@@ -3543,7 +3541,7 @@
         <v>2</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F78" s="71"/>
       <c r="G78" s="71"/>
@@ -3568,15 +3566,15 @@
     </row>
     <row r="81" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E81" s="2"/>
       <c r="L81" s="43" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3584,16 +3582,16 @@
         <v>19</v>
       </c>
       <c r="B82" s="45" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C82" s="45" t="s">
         <v>13</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E82" s="45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F82" s="45" t="s">
         <v>14</v>
@@ -3611,7 +3609,7 @@
         <v>19</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="N82" s="2" t="s">
         <v>10</v>
@@ -3813,7 +3811,7 @@
     </row>
     <row r="90" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E90" s="2"/>
     </row>
@@ -3822,7 +3820,7 @@
         <v>19</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E91" s="2"/>
     </row>
@@ -3840,7 +3838,7 @@
     </row>
     <row r="95" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="44" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E95" s="2"/>
     </row>
@@ -3849,16 +3847,16 @@
         <v>19</v>
       </c>
       <c r="B96" s="45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C96" s="45" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D96" s="45" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E96" s="45" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -9384,9 +9382,9 @@
     <mergeCell ref="A13:B13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E67" r:id="rId1"/>
-    <hyperlink ref="E68" r:id="rId2"/>
-    <hyperlink ref="E70" r:id="rId3"/>
+    <hyperlink ref="G67" r:id="rId1"/>
+    <hyperlink ref="G68" r:id="rId2"/>
+    <hyperlink ref="G70" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>

</xml_diff>